<commit_message>
Varios. Mensaje de error en ATV incorrecto y import productos y proveedores
</commit_message>
<xml_diff>
--- a/public/assets/files/PlantillaProveedores.xlsx
+++ b/public/assets/files/PlantillaProveedores.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissa/Dropbox/phormo/etax/plantillas excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FE3CF1-E6A5-BF41-BB74-03F06FA9AADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE7D099-0BAB-49E5-B158-A504B7E2D6CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Proveedores" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -109,66 +109,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">1 - Cédula física
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">2 - Cédula jurídica
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">3 - DIMEX
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">4 - NITE
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">5 - Extranjero
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>6 - Otro</t>
+F - Cédula física
+J - Cédula jurídica
+D - DIMEX
+N - NITE
+E - Extranjero
+O - Otro</t>
         </r>
       </text>
     </comment>
@@ -790,7 +736,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Codigo</t>
   </si>
@@ -843,18 +789,9 @@
     <t>AreaTel</t>
   </si>
   <si>
-    <t>Exento</t>
-  </si>
-  <si>
-    <t>EmisorReceptor</t>
-  </si>
-  <si>
     <t>CR</t>
   </si>
   <si>
-    <t>CODEJ</t>
-  </si>
-  <si>
     <t>Apelllido1</t>
   </si>
   <si>
@@ -870,16 +807,7 @@
     <t>1234-1234</t>
   </si>
   <si>
-    <t>XXXXXXXXX</t>
-  </si>
-  <si>
     <t>Indique el número de teléfono</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <r>
@@ -949,10 +877,10 @@
     <t>Indique una dirección de correo electrónico adicional del proveedor.</t>
   </si>
   <si>
-    <t>Elija la opción que indica si el proveedor regularmente está exento (SÍ) o no (NO)</t>
-  </si>
-  <si>
-    <t>Indique si el proveedor es emisor (E), receptor (R), o emisor y receptor de facturación electrónia (ER)</t>
+    <t>F</t>
+  </si>
+  <si>
+    <t>CODEJ</t>
   </si>
 </sst>
 </file>
@@ -1034,15 +962,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1052,13 +974,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1075,9 +1000,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:R4">
-  <autoFilter ref="A3:R4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:P4">
+  <autoFilter ref="A3:P4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Codigo"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nombre"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PrimerApellido"/>
@@ -1094,15 +1019,13 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="AreaTel"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Telefono"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CorreosCopia"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Exento"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="EmisorReceptor"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1398,101 +1321,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="18" width="20.83203125" customWidth="1"/>
+    <col min="1" max="16" width="20.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" ht="65" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+    </row>
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1541,37 +1456,31 @@
       <c r="P3" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" t="s">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="5">
+        <v>111111111</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
-      </c>
-      <c r="R3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1586,37 +1495,25 @@
         <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N4" t="s">
         <v>9</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A1:U1"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{FB5AAD66-7B56-EC41-89B1-925E7155AB49}">
-      <formula1>"1, 2, 3, 4, 5, 6"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R4" xr:uid="{FD64E9DF-C202-6D40-8A35-F9E0D6012FAE}">
-      <formula1>"E,R,ER"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4" xr:uid="{3F792A50-2C73-3045-9F03-4CB2152D0231}">
-      <formula1>"SÍ,NO"</formula1>
+      <formula1>"F, J, D, N, E, O"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1624,9 +1521,10 @@
     <hyperlink ref="P4" r:id="rId2" xr:uid="{FFE41E9D-3233-495D-BE64-74207D3A2BEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>